<commit_message>
Cell/column type example sheet; use in vignette
</commit_message>
<xml_diff>
--- a/inst/extdata/deaths.xlsx
+++ b/inst/extdata/deaths.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="arts" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>Lots of people</t>
   </si>
@@ -126,9 +126,6 @@
     <t>too!</t>
   </si>
   <si>
-    <t>at the bottom,</t>
-  </si>
-  <si>
     <t>Mohamed Ali</t>
   </si>
   <si>
@@ -223,6 +220,15 @@
   </si>
   <si>
     <t>up here.</t>
+  </si>
+  <si>
+    <t>Has kids</t>
+  </si>
+  <si>
+    <t>at the</t>
+  </si>
+  <si>
+    <t>bottom,</t>
   </si>
 </sst>
 </file>
@@ -293,14 +299,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:E15" totalsRowShown="0">
-  <autoFilter ref="A5:E15"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:F15" totalsRowShown="0">
+  <autoFilter ref="A5:F15"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Profession"/>
     <tableColumn id="5" name="Age">
-      <calculatedColumnFormula>DATEDIF(D6,E6,"y")</calculatedColumnFormula>
+      <calculatedColumnFormula>DATEDIF(E6,F6,"y")</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="6" name="Has kids"/>
     <tableColumn id="3" name="Date of birth" dataDxfId="3"/>
     <tableColumn id="4" name="Date of death" dataDxfId="2"/>
   </tableColumns>
@@ -309,14 +316,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A5:E15" totalsRowShown="0">
-  <autoFilter ref="A5:E15"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A5:F15" totalsRowShown="0">
+  <autoFilter ref="A5:F15"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Profession"/>
     <tableColumn id="5" name="Age">
-      <calculatedColumnFormula>DATEDIF(D6,E6,"y")</calculatedColumnFormula>
+      <calculatedColumnFormula>DATEDIF(E6,F6,"y")</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="6" name="Has kids"/>
     <tableColumn id="3" name="Date of birth" dataDxfId="1"/>
     <tableColumn id="4" name="Date of death" dataDxfId="0"/>
   </tableColumns>
@@ -587,35 +595,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" zoomScalePageLayoutView="157" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD15"/>
+    <sheetView zoomScale="157" zoomScaleNormal="157" zoomScalePageLayoutView="157" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -625,14 +634,14 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -641,11 +650,12 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -656,13 +666,16 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -670,17 +683,20 @@
         <v>16</v>
       </c>
       <c r="C6">
-        <f>DATEDIF(D6,E6,"y")</f>
+        <f t="shared" ref="C6:C15" si="0">DATEDIF(E6,F6,"y")</f>
         <v>69</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
         <v>17175</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>42379</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -688,17 +704,20 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <f>DATEDIF(D7,E7,"y")</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
         <v>20749</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>42731</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -706,17 +725,20 @@
         <v>16</v>
       </c>
       <c r="C8">
-        <f>DATEDIF(D8,E8,"y")</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
         <v>9788</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>42812</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -724,17 +746,20 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <f>DATEDIF(D9,E9,"y")</f>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
         <v>20226</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>42791</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -742,17 +767,20 @@
         <v>16</v>
       </c>
       <c r="C10">
-        <f>DATEDIF(D10,E10,"y")</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
         <v>21343</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>42481</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -760,17 +788,20 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <f>DATEDIF(D11,E11,"y")</f>
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
         <v>16854</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>42383</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -778,17 +809,20 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <f>DATEDIF(D12,E12,"y")</f>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
         <v>12464</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>42698</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -796,17 +830,20 @@
         <v>27</v>
       </c>
       <c r="C13">
-        <f>DATEDIF(D13,E13,"y")</f>
+        <f t="shared" si="0"/>
         <v>89</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
         <v>9615</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>42419</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -814,17 +851,20 @@
         <v>11</v>
       </c>
       <c r="C14">
-        <f>DATEDIF(D14,E14,"y")</f>
+        <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
         <v>6247</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>42722</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -832,39 +872,45 @@
         <v>16</v>
       </c>
       <c r="C15">
-        <f>DATEDIF(D15,E15,"y")</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
         <v>23187</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>42729</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -875,60 +921,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView zoomScale="217" zoomScaleNormal="217" zoomScalePageLayoutView="217" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" zoomScale="217" zoomScaleNormal="217" zoomScalePageLayoutView="217" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="5.5" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="3" max="4" width="5.5" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
         <v>51</v>
       </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="2"/>
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -939,220 +986,253 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
       <c r="C6">
-        <f t="shared" ref="C6:C15" si="0">DATEDIF(D6,E6,"y")</f>
+        <f t="shared" ref="C6:C15" si="0">DATEDIF(E6,F6,"y")</f>
         <v>88</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
         <v>10432</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>42729</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>15358</v>
+      </c>
+      <c r="F7" s="1">
+        <v>42524</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="D7" s="1">
-        <v>15358</v>
-      </c>
-      <c r="E7" s="1">
-        <v>42524</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>11635</v>
+      </c>
+      <c r="F8" s="1">
+        <v>42509</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>9722</v>
+      </c>
+      <c r="F9" s="1">
+        <v>42699</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>13220</v>
+      </c>
+      <c r="F10" s="1">
+        <v>42413</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>39</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>84</v>
-      </c>
-      <c r="D8" s="1">
-        <v>11635</v>
-      </c>
-      <c r="E8" s="1">
-        <v>42509</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>27202</v>
+      </c>
+      <c r="F11" s="1">
+        <v>42537</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>14082</v>
+      </c>
+      <c r="F12" s="1">
+        <v>42681</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>20361</v>
+      </c>
+      <c r="F13" s="1">
+        <v>42688</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>7880</v>
+      </c>
+      <c r="F14" s="1">
+        <v>42712</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
         <v>46</v>
       </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="D9" s="1">
-        <v>9722</v>
-      </c>
-      <c r="E9" s="1">
-        <v>42699</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
-      <c r="D10" s="1">
-        <v>13220</v>
-      </c>
-      <c r="E10" s="1">
-        <v>42413</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="D11" s="1">
-        <v>27202</v>
-      </c>
-      <c r="E11" s="1">
-        <v>42537</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>78</v>
-      </c>
-      <c r="D12" s="1">
-        <v>14082</v>
-      </c>
-      <c r="E12" s="1">
-        <v>42681</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>19159</v>
+      </c>
+      <c r="F15" s="1">
+        <v>42549</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="1">
-        <v>20361</v>
-      </c>
-      <c r="E13" s="1">
-        <v>42688</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>95</v>
-      </c>
-      <c r="D14" s="1">
-        <v>7880</v>
-      </c>
-      <c r="E14" s="1">
-        <v>42712</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="D15" s="1">
-        <v>19159</v>
-      </c>
-      <c r="E15" s="1">
-        <v>42549</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="E19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Cell and column type vignette (#332)
* init two more vignettes

* Stub out sheet geometry vignette; re-pkgdown

* First draft cell/column typing vignette

* Act on @hadley feedback

* Cell/column type example sheet; use in vignette

* Update workflows article for new column in deaths.xlsx

* Label the true setup chunk
</commit_message>
<xml_diff>
--- a/inst/extdata/deaths.xlsx
+++ b/inst/extdata/deaths.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="arts" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>Lots of people</t>
   </si>
@@ -126,9 +126,6 @@
     <t>too!</t>
   </si>
   <si>
-    <t>at the bottom,</t>
-  </si>
-  <si>
     <t>Mohamed Ali</t>
   </si>
   <si>
@@ -223,6 +220,15 @@
   </si>
   <si>
     <t>up here.</t>
+  </si>
+  <si>
+    <t>Has kids</t>
+  </si>
+  <si>
+    <t>at the</t>
+  </si>
+  <si>
+    <t>bottom,</t>
   </si>
 </sst>
 </file>
@@ -293,14 +299,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:E15" totalsRowShown="0">
-  <autoFilter ref="A5:E15"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:F15" totalsRowShown="0">
+  <autoFilter ref="A5:F15"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Profession"/>
     <tableColumn id="5" name="Age">
-      <calculatedColumnFormula>DATEDIF(D6,E6,"y")</calculatedColumnFormula>
+      <calculatedColumnFormula>DATEDIF(E6,F6,"y")</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="6" name="Has kids"/>
     <tableColumn id="3" name="Date of birth" dataDxfId="3"/>
     <tableColumn id="4" name="Date of death" dataDxfId="2"/>
   </tableColumns>
@@ -309,14 +316,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A5:E15" totalsRowShown="0">
-  <autoFilter ref="A5:E15"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A5:F15" totalsRowShown="0">
+  <autoFilter ref="A5:F15"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Profession"/>
     <tableColumn id="5" name="Age">
-      <calculatedColumnFormula>DATEDIF(D6,E6,"y")</calculatedColumnFormula>
+      <calculatedColumnFormula>DATEDIF(E6,F6,"y")</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="6" name="Has kids"/>
     <tableColumn id="3" name="Date of birth" dataDxfId="1"/>
     <tableColumn id="4" name="Date of death" dataDxfId="0"/>
   </tableColumns>
@@ -587,35 +595,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" zoomScalePageLayoutView="157" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD15"/>
+    <sheetView zoomScale="157" zoomScaleNormal="157" zoomScalePageLayoutView="157" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -625,14 +634,14 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -641,11 +650,12 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -656,13 +666,16 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -670,17 +683,20 @@
         <v>16</v>
       </c>
       <c r="C6">
-        <f>DATEDIF(D6,E6,"y")</f>
+        <f t="shared" ref="C6:C15" si="0">DATEDIF(E6,F6,"y")</f>
         <v>69</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
         <v>17175</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>42379</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -688,17 +704,20 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <f>DATEDIF(D7,E7,"y")</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
         <v>20749</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>42731</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -706,17 +725,20 @@
         <v>16</v>
       </c>
       <c r="C8">
-        <f>DATEDIF(D8,E8,"y")</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
         <v>9788</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>42812</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -724,17 +746,20 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <f>DATEDIF(D9,E9,"y")</f>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
         <v>20226</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>42791</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -742,17 +767,20 @@
         <v>16</v>
       </c>
       <c r="C10">
-        <f>DATEDIF(D10,E10,"y")</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
         <v>21343</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>42481</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -760,17 +788,20 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <f>DATEDIF(D11,E11,"y")</f>
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
         <v>16854</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>42383</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -778,17 +809,20 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <f>DATEDIF(D12,E12,"y")</f>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
         <v>12464</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>42698</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -796,17 +830,20 @@
         <v>27</v>
       </c>
       <c r="C13">
-        <f>DATEDIF(D13,E13,"y")</f>
+        <f t="shared" si="0"/>
         <v>89</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
         <v>9615</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>42419</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -814,17 +851,20 @@
         <v>11</v>
       </c>
       <c r="C14">
-        <f>DATEDIF(D14,E14,"y")</f>
+        <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
         <v>6247</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>42722</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -832,39 +872,45 @@
         <v>16</v>
       </c>
       <c r="C15">
-        <f>DATEDIF(D15,E15,"y")</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
         <v>23187</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>42729</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -875,60 +921,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView zoomScale="217" zoomScaleNormal="217" zoomScalePageLayoutView="217" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" zoomScale="217" zoomScaleNormal="217" zoomScalePageLayoutView="217" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="5.5" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="3" max="4" width="5.5" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" t="s">
         <v>51</v>
       </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" s="2"/>
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -939,220 +986,253 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
       <c r="C6">
-        <f t="shared" ref="C6:C15" si="0">DATEDIF(D6,E6,"y")</f>
+        <f t="shared" ref="C6:C15" si="0">DATEDIF(E6,F6,"y")</f>
         <v>88</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
         <v>10432</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>42729</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>15358</v>
+      </c>
+      <c r="F7" s="1">
+        <v>42524</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="D7" s="1">
-        <v>15358</v>
-      </c>
-      <c r="E7" s="1">
-        <v>42524</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>11635</v>
+      </c>
+      <c r="F8" s="1">
+        <v>42509</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>9722</v>
+      </c>
+      <c r="F9" s="1">
+        <v>42699</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>13220</v>
+      </c>
+      <c r="F10" s="1">
+        <v>42413</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>39</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>84</v>
-      </c>
-      <c r="D8" s="1">
-        <v>11635</v>
-      </c>
-      <c r="E8" s="1">
-        <v>42509</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>27202</v>
+      </c>
+      <c r="F11" s="1">
+        <v>42537</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>14082</v>
+      </c>
+      <c r="F12" s="1">
+        <v>42681</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>20361</v>
+      </c>
+      <c r="F13" s="1">
+        <v>42688</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>7880</v>
+      </c>
+      <c r="F14" s="1">
+        <v>42712</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
         <v>46</v>
       </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="D9" s="1">
-        <v>9722</v>
-      </c>
-      <c r="E9" s="1">
-        <v>42699</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
-      <c r="D10" s="1">
-        <v>13220</v>
-      </c>
-      <c r="E10" s="1">
-        <v>42413</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="D11" s="1">
-        <v>27202</v>
-      </c>
-      <c r="E11" s="1">
-        <v>42537</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>78</v>
-      </c>
-      <c r="D12" s="1">
-        <v>14082</v>
-      </c>
-      <c r="E12" s="1">
-        <v>42681</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>19159</v>
+      </c>
+      <c r="F15" s="1">
+        <v>42549</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="1">
-        <v>20361</v>
-      </c>
-      <c r="E13" s="1">
-        <v>42688</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>95</v>
-      </c>
-      <c r="D14" s="1">
-        <v>7880</v>
-      </c>
-      <c r="E14" s="1">
-        <v>42712</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="D15" s="1">
-        <v>19159</v>
-      </c>
-      <c r="E15" s="1">
-        <v>42549</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="E19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>